<commit_message>
Exercise 6 and 7
</commit_message>
<xml_diff>
--- a/examplesheet/example.xlsx
+++ b/examplesheet/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CS317813\PycharmProjects\ExcelPrototyping\examplesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricku\PycharmProjects\ExcelPrototyping\examplesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D17B482-0C72-4511-BED7-FD90F8D08BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4CEA27-3420-4871-A7B4-D5EE497A8B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CEBC942-0CB9-402A-9791-B1E5E7477842}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2CEBC942-0CB9-402A-9791-B1E5E7477842}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>LOTE</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Chamado</t>
+  </si>
+  <si>
+    <t>06/02 - TICKET00001
+06-02 - TICKET00001
+RITM000TESTE2
+RITM000TESTE</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,6 +331,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,14 +664,14 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -754,6 +763,9 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
+      <c r="N2" s="15" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:14" s="11" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">

</xml_diff>